<commit_message>
Edit offertes after feedback
</commit_message>
<xml_diff>
--- a/opdracht03/documentatie/Offerte groep 36.xlsx
+++ b/opdracht03/documentatie/Offerte groep 36.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\2\Vakken\Projecten 2\p2ops-g10\opdracht03\documentatie\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94E7A3E2-F351-4B7E-BC4E-BBC030CA2941}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FB86883-A5CD-4CB5-AD95-444B1A95B64D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2673" yWindow="1440" windowWidth="19200" windowHeight="10073" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13986" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Meerdere pagina's" sheetId="4" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="51">
   <si>
     <t>Offerte</t>
   </si>
@@ -169,6 +169,21 @@
   </si>
   <si>
     <t>VoIP Telenet FreePhone Business abonnement per gebruiker - 1 jaar</t>
+  </si>
+  <si>
+    <t>Newstar NM-C440 TV Beugel</t>
+  </si>
+  <si>
+    <t>Finlux FL4022 - Full HD TV</t>
+  </si>
+  <si>
+    <t>Samsung Gear 360 Camera</t>
+  </si>
+  <si>
+    <t>Licenties</t>
+  </si>
+  <si>
+    <t>Omnicasa</t>
   </si>
 </sst>
 </file>
@@ -474,7 +489,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="83">
+  <cellXfs count="89">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -614,8 +629,49 @@
     <xf numFmtId="164" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -630,55 +686,30 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="5" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -694,7 +725,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1014,10 +1045,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I63"/>
+  <dimension ref="A1:I67"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A35" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A48" sqref="A48:B48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1171875" defaultRowHeight="11.35" x14ac:dyDescent="0.35"/>
@@ -1051,10 +1082,10 @@
       <c r="C3" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="63" t="s">
+      <c r="D3" s="78" t="s">
         <v>32</v>
       </c>
-      <c r="E3" s="64"/>
+      <c r="E3" s="79"/>
       <c r="F3" s="21" t="s">
         <v>3</v>
       </c>
@@ -1069,10 +1100,10 @@
       <c r="C4" s="37">
         <v>43605</v>
       </c>
-      <c r="D4" s="65" t="s">
+      <c r="D4" s="80" t="s">
         <v>40</v>
       </c>
-      <c r="E4" s="66"/>
+      <c r="E4" s="81"/>
       <c r="F4" s="38" t="s">
         <v>41</v>
       </c>
@@ -1086,10 +1117,10 @@
       <c r="F5" s="17"/>
     </row>
     <row r="6" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" s="70" t="s">
+      <c r="A6" s="65" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="70"/>
+      <c r="B6" s="65"/>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
@@ -1104,10 +1135,10 @@
       <c r="F7" s="4"/>
     </row>
     <row r="8" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="71" t="s">
+      <c r="A8" s="74" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="71"/>
+      <c r="B8" s="74"/>
       <c r="C8" s="21" t="s">
         <v>12</v>
       </c>
@@ -1122,10 +1153,10 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="67" t="s">
+      <c r="A9" s="63" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="68"/>
+      <c r="B9" s="64"/>
       <c r="C9" s="5">
         <v>1</v>
       </c>
@@ -1141,10 +1172,10 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="67" t="s">
+      <c r="A10" s="63" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="68"/>
+      <c r="B10" s="64"/>
       <c r="C10" s="5">
         <v>1</v>
       </c>
@@ -1160,10 +1191,10 @@
       </c>
     </row>
     <row r="11" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="67" t="s">
+      <c r="A11" s="63" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="68"/>
+      <c r="B11" s="64"/>
       <c r="C11" s="5">
         <v>1</v>
       </c>
@@ -1179,10 +1210,10 @@
       </c>
     </row>
     <row r="12" spans="1:6" s="58" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="67" t="s">
+      <c r="A12" s="63" t="s">
         <v>38</v>
       </c>
-      <c r="B12" s="68"/>
+      <c r="B12" s="64"/>
       <c r="C12" s="5">
         <v>1</v>
       </c>
@@ -1198,10 +1229,10 @@
       </c>
     </row>
     <row r="13" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="67" t="s">
+      <c r="A13" s="63" t="s">
         <v>28</v>
       </c>
-      <c r="B13" s="68"/>
+      <c r="B13" s="64"/>
       <c r="C13" s="5">
         <v>1</v>
       </c>
@@ -1217,10 +1248,10 @@
       </c>
     </row>
     <row r="14" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="67" t="s">
+      <c r="A14" s="63" t="s">
         <v>25</v>
       </c>
-      <c r="B14" s="68"/>
+      <c r="B14" s="64"/>
       <c r="C14" s="5">
         <v>2</v>
       </c>
@@ -1236,10 +1267,10 @@
       </c>
     </row>
     <row r="15" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="67" t="s">
+      <c r="A15" s="63" t="s">
         <v>26</v>
       </c>
-      <c r="B15" s="68"/>
+      <c r="B15" s="64"/>
       <c r="C15" s="5">
         <v>2</v>
       </c>
@@ -1255,10 +1286,10 @@
       </c>
     </row>
     <row r="16" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="67" t="s">
+      <c r="A16" s="63" t="s">
         <v>39</v>
       </c>
-      <c r="B16" s="68"/>
+      <c r="B16" s="64"/>
       <c r="C16" s="5">
         <v>1</v>
       </c>
@@ -1274,10 +1305,10 @@
       </c>
     </row>
     <row r="17" spans="1:9" s="59" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="75" t="s">
+      <c r="A17" s="67" t="s">
         <v>27</v>
       </c>
-      <c r="B17" s="81"/>
+      <c r="B17" s="68"/>
       <c r="C17" s="31">
         <v>3</v>
       </c>
@@ -1302,10 +1333,10 @@
       <c r="F18" s="25"/>
     </row>
     <row r="19" spans="1:9" s="27" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A19" s="70" t="s">
+      <c r="A19" s="65" t="s">
         <v>29</v>
       </c>
-      <c r="B19" s="70"/>
+      <c r="B19" s="65"/>
       <c r="C19" s="30"/>
       <c r="D19" s="12"/>
       <c r="E19" s="13"/>
@@ -1323,10 +1354,10 @@
       <c r="I20" s="14"/>
     </row>
     <row r="21" spans="1:9" ht="14.7" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="71" t="s">
+      <c r="A21" s="74" t="s">
         <v>10</v>
       </c>
-      <c r="B21" s="71"/>
+      <c r="B21" s="74"/>
       <c r="C21" s="41" t="s">
         <v>30</v>
       </c>
@@ -1341,10 +1372,10 @@
       </c>
     </row>
     <row r="22" spans="1:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="79" t="s">
+      <c r="A22" s="72" t="s">
         <v>44</v>
       </c>
-      <c r="B22" s="80"/>
+      <c r="B22" s="73"/>
       <c r="C22" s="52">
         <v>40</v>
       </c>
@@ -1360,24 +1391,24 @@
       </c>
     </row>
     <row r="23" spans="1:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="67"/>
-      <c r="B23" s="68"/>
+      <c r="A23" s="63"/>
+      <c r="B23" s="64"/>
       <c r="C23" s="50"/>
       <c r="D23" s="49"/>
       <c r="E23" s="7"/>
       <c r="F23" s="51"/>
     </row>
     <row r="24" spans="1:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="75"/>
-      <c r="B24" s="76"/>
+      <c r="A24" s="67"/>
+      <c r="B24" s="83"/>
       <c r="C24" s="57"/>
       <c r="D24" s="44"/>
       <c r="E24" s="33"/>
       <c r="F24" s="56"/>
     </row>
     <row r="25" spans="1:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="69"/>
-      <c r="B25" s="69"/>
+      <c r="A25" s="82"/>
+      <c r="B25" s="82"/>
       <c r="C25" s="24"/>
       <c r="D25" s="12"/>
       <c r="E25" s="13"/>
@@ -1392,11 +1423,11 @@
       <c r="F26" s="25"/>
     </row>
     <row r="27" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="82" t="s">
+      <c r="A27" s="69" t="s">
         <v>34</v>
       </c>
-      <c r="B27" s="82"/>
-      <c r="C27" s="82"/>
+      <c r="B27" s="69"/>
+      <c r="C27" s="69"/>
       <c r="D27" s="12"/>
       <c r="E27" s="13"/>
       <c r="F27" s="25"/>
@@ -1410,10 +1441,10 @@
       <c r="F28" s="25"/>
     </row>
     <row r="29" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="71" t="s">
+      <c r="A29" s="74" t="s">
         <v>10</v>
       </c>
-      <c r="B29" s="71"/>
+      <c r="B29" s="74"/>
       <c r="C29" s="21" t="s">
         <v>12</v>
       </c>
@@ -1428,10 +1459,10 @@
       </c>
     </row>
     <row r="30" spans="1:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="67" t="s">
+      <c r="A30" s="63" t="s">
         <v>19</v>
       </c>
-      <c r="B30" s="68"/>
+      <c r="B30" s="64"/>
       <c r="C30" s="5">
         <v>2</v>
       </c>
@@ -1447,10 +1478,10 @@
       </c>
     </row>
     <row r="31" spans="1:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="67" t="s">
+      <c r="A31" s="63" t="s">
         <v>16</v>
       </c>
-      <c r="B31" s="68"/>
+      <c r="B31" s="64"/>
       <c r="C31" s="5">
         <v>2</v>
       </c>
@@ -1466,10 +1497,10 @@
       </c>
     </row>
     <row r="32" spans="1:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="67" t="s">
+      <c r="A32" s="63" t="s">
         <v>17</v>
       </c>
-      <c r="B32" s="68"/>
+      <c r="B32" s="64"/>
       <c r="C32" s="5">
         <v>2</v>
       </c>
@@ -1485,10 +1516,10 @@
       </c>
     </row>
     <row r="33" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="67" t="s">
+      <c r="A33" s="63" t="s">
         <v>18</v>
       </c>
-      <c r="B33" s="68"/>
+      <c r="B33" s="64"/>
       <c r="C33" s="5">
         <v>2</v>
       </c>
@@ -1499,15 +1530,15 @@
         <v>0.21</v>
       </c>
       <c r="F33" s="8">
-        <f t="shared" ref="F33:F39" si="1">SUM(C33*D33)</f>
+        <f t="shared" ref="F33:F42" si="1">SUM(C33*D33)</f>
         <v>19.8</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="67" t="s">
+      <c r="A34" s="63" t="s">
         <v>43</v>
       </c>
-      <c r="B34" s="68"/>
+      <c r="B34" s="64"/>
       <c r="C34" s="5">
         <v>1</v>
       </c>
@@ -1523,10 +1554,10 @@
       </c>
     </row>
     <row r="35" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="67" t="s">
+      <c r="A35" s="63" t="s">
         <v>20</v>
       </c>
-      <c r="B35" s="68"/>
+      <c r="B35" s="64"/>
       <c r="C35" s="5">
         <v>1</v>
       </c>
@@ -1542,10 +1573,10 @@
       </c>
     </row>
     <row r="36" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="67" t="s">
+      <c r="A36" s="63" t="s">
         <v>35</v>
       </c>
-      <c r="B36" s="68"/>
+      <c r="B36" s="64"/>
       <c r="C36" s="5">
         <v>1</v>
       </c>
@@ -1561,10 +1592,10 @@
       </c>
     </row>
     <row r="37" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="67" t="s">
+      <c r="A37" s="63" t="s">
         <v>21</v>
       </c>
-      <c r="B37" s="68"/>
+      <c r="B37" s="64"/>
       <c r="C37" s="5">
         <v>1</v>
       </c>
@@ -1579,221 +1610,315 @@
         <v>65</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="67" t="s">
-        <v>45</v>
-      </c>
-      <c r="B38" s="68"/>
+    <row r="38" spans="1:6" s="61" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A38" s="63" t="s">
+        <v>47</v>
+      </c>
+      <c r="B38" s="64"/>
       <c r="C38" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D38" s="6">
-        <v>198</v>
+        <v>165.3</v>
       </c>
       <c r="E38" s="7">
         <v>0.21</v>
       </c>
       <c r="F38" s="8">
         <f t="shared" si="1"/>
-        <v>396</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="67" t="s">
-        <v>42</v>
-      </c>
-      <c r="B39" s="68"/>
+        <v>165.3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" s="61" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A39" s="63" t="s">
+        <v>48</v>
+      </c>
+      <c r="B39" s="64"/>
       <c r="C39" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D39" s="6">
-        <v>49.5</v>
+        <v>100.4</v>
       </c>
       <c r="E39" s="7">
         <v>0.21</v>
       </c>
       <c r="F39" s="8">
         <f t="shared" si="1"/>
+        <v>100.4</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" s="61" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A40" s="63" t="s">
+        <v>46</v>
+      </c>
+      <c r="B40" s="64"/>
+      <c r="C40" s="5">
+        <v>1</v>
+      </c>
+      <c r="D40" s="6">
+        <v>82.6</v>
+      </c>
+      <c r="E40" s="7">
+        <v>0.21</v>
+      </c>
+      <c r="F40" s="8">
+        <f t="shared" si="1"/>
+        <v>82.6</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A41" s="63" t="s">
+        <v>45</v>
+      </c>
+      <c r="B41" s="64"/>
+      <c r="C41" s="5">
+        <v>2</v>
+      </c>
+      <c r="D41" s="6">
+        <v>198</v>
+      </c>
+      <c r="E41" s="7">
+        <v>0.21</v>
+      </c>
+      <c r="F41" s="8">
+        <f t="shared" si="1"/>
+        <v>396</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A42" s="63" t="s">
+        <v>42</v>
+      </c>
+      <c r="B42" s="64"/>
+      <c r="C42" s="5">
+        <v>2</v>
+      </c>
+      <c r="D42" s="6">
+        <v>49.5</v>
+      </c>
+      <c r="E42" s="7">
+        <v>0.21</v>
+      </c>
+      <c r="F42" s="8">
+        <f t="shared" si="1"/>
         <v>99</v>
       </c>
     </row>
-    <row r="40" spans="1:6" s="42" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="67" t="s">
+    <row r="43" spans="1:6" s="42" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A43" s="63" t="s">
         <v>36</v>
       </c>
-      <c r="B40" s="72"/>
-      <c r="C40" s="5">
+      <c r="B43" s="66"/>
+      <c r="C43" s="5">
         <v>2</v>
       </c>
-      <c r="D40" s="6">
+      <c r="D43" s="6">
         <v>7.4</v>
       </c>
-      <c r="E40" s="47">
-        <v>0.21</v>
-      </c>
-      <c r="F40" s="8">
-        <f>SUM(C40*D40)</f>
+      <c r="E43" s="47">
+        <v>0.21</v>
+      </c>
+      <c r="F43" s="8">
+        <f>SUM(C43*D43)</f>
         <v>14.8</v>
       </c>
     </row>
-    <row r="41" spans="1:6" s="42" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="75" t="s">
+    <row r="44" spans="1:6" s="42" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A44" s="67" t="s">
         <v>37</v>
       </c>
-      <c r="B41" s="81"/>
-      <c r="C41" s="31">
+      <c r="B44" s="68"/>
+      <c r="C44" s="31">
         <v>1</v>
       </c>
-      <c r="D41" s="32">
+      <c r="D44" s="32">
         <v>2.4500000000000002</v>
       </c>
-      <c r="E41" s="48">
-        <v>0.21</v>
-      </c>
-      <c r="F41" s="34">
-        <f>SUM(C41*D41)</f>
+      <c r="E44" s="48">
+        <v>0.21</v>
+      </c>
+      <c r="F44" s="34">
+        <f>SUM(C44*D44)</f>
         <v>2.4500000000000002</v>
       </c>
     </row>
-    <row r="42" spans="1:6" s="27" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="F42" s="25"/>
-    </row>
-    <row r="43" spans="1:6" s="28" customFormat="1" ht="37.35" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="61"/>
-      <c r="B43" s="61"/>
-      <c r="C43" s="30"/>
-      <c r="D43" s="12"/>
-      <c r="E43" s="13"/>
-      <c r="F43" s="25"/>
-    </row>
-    <row r="44" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="72"/>
-      <c r="B44" s="72"/>
-      <c r="C44" s="30"/>
-      <c r="D44" s="12"/>
-      <c r="E44" s="13"/>
-      <c r="F44" s="25"/>
-    </row>
-    <row r="45" spans="1:6" ht="37.35" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A45" s="72"/>
-      <c r="B45" s="72"/>
-      <c r="C45" s="30"/>
-      <c r="D45" s="12"/>
-      <c r="E45" s="13"/>
+    <row r="45" spans="1:6" s="27" customFormat="1" ht="13.35" customHeight="1" x14ac:dyDescent="0.35">
       <c r="F45" s="25"/>
     </row>
-    <row r="46" spans="1:6" ht="14" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A46" s="4"/>
-      <c r="B46" s="4"/>
-      <c r="C46" s="4"/>
-      <c r="D46" s="4"/>
-      <c r="E46" s="4"/>
-      <c r="F46" s="4"/>
-    </row>
-    <row r="47" spans="1:6" s="27" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A47" s="4"/>
-      <c r="B47" s="4"/>
-      <c r="C47" s="4"/>
-      <c r="D47" s="4"/>
-      <c r="E47" s="4"/>
-      <c r="F47" s="4"/>
-    </row>
-    <row r="48" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="D48" s="73" t="s">
+    <row r="46" spans="1:6" s="28" customFormat="1" ht="15.35" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A46" s="69" t="s">
+        <v>49</v>
+      </c>
+      <c r="B46" s="69"/>
+      <c r="C46" s="30"/>
+      <c r="D46" s="12"/>
+      <c r="E46" s="13"/>
+      <c r="F46" s="25"/>
+    </row>
+    <row r="47" spans="1:6" s="61" customFormat="1" ht="15.35" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A47" s="62"/>
+      <c r="B47" s="62"/>
+      <c r="C47" s="30"/>
+      <c r="D47" s="12"/>
+      <c r="E47" s="13"/>
+      <c r="F47" s="25"/>
+    </row>
+    <row r="48" spans="1:6" ht="13.7" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A48" s="84" t="s">
+        <v>10</v>
+      </c>
+      <c r="B48" s="88"/>
+      <c r="C48" s="87" t="s">
+        <v>12</v>
+      </c>
+      <c r="D48" s="85" t="s">
+        <v>11</v>
+      </c>
+      <c r="E48" s="86" t="s">
+        <v>4</v>
+      </c>
+      <c r="F48" s="85" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" ht="37.35" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A49" s="67" t="s">
+        <v>50</v>
+      </c>
+      <c r="B49" s="83"/>
+      <c r="C49" s="57">
+        <v>2</v>
+      </c>
+      <c r="D49" s="44">
+        <v>0</v>
+      </c>
+      <c r="E49" s="33">
+        <v>0.21</v>
+      </c>
+      <c r="F49" s="56">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" ht="14" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A50" s="4"/>
+      <c r="B50" s="4"/>
+      <c r="C50" s="4"/>
+      <c r="D50" s="4"/>
+      <c r="E50" s="4"/>
+      <c r="F50" s="4"/>
+    </row>
+    <row r="51" spans="1:6" s="27" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A51" s="4"/>
+      <c r="B51" s="4"/>
+      <c r="C51" s="4"/>
+      <c r="D51" s="4"/>
+      <c r="E51" s="4"/>
+      <c r="F51" s="4"/>
+    </row>
+    <row r="52" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D52" s="75" t="s">
         <v>33</v>
       </c>
-      <c r="E48" s="74"/>
-      <c r="F48" s="45">
-        <f>SUM(F9:F46)</f>
-        <v>5811.6100000000006</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="D49" s="73" t="s">
+      <c r="E52" s="76"/>
+      <c r="F52" s="45">
+        <f>SUM(F9:F50)</f>
+        <v>6159.9100000000008</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D53" s="75" t="s">
         <v>8</v>
       </c>
-      <c r="E49" s="74"/>
-      <c r="F49" s="45">
-        <f>SUMIF(E9:E45,"=21%",F9:F45)/100*21</f>
-        <v>1220.4381000000001</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="D50" s="73" t="s">
+      <c r="E53" s="76"/>
+      <c r="F53" s="45">
+        <f>SUMIF(E9:E49,"=21%",F9:F49)/100*21</f>
+        <v>1293.5811000000001</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D54" s="75" t="s">
         <v>6</v>
       </c>
-      <c r="E50" s="74"/>
-      <c r="F50" s="45">
-        <f>SUMIF(E9:E45,"=6%",F9:F45)/100*6</f>
+      <c r="E54" s="76"/>
+      <c r="F54" s="45">
+        <f>SUMIF(E9:E49,"=6%",F9:F49)/100*6</f>
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:6" ht="18" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="D51" s="77" t="s">
+    <row r="55" spans="1:6" ht="18" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D55" s="70" t="s">
         <v>7</v>
       </c>
-      <c r="E51" s="78"/>
-      <c r="F51" s="46">
-        <f>SUM(F48+F49+F50)</f>
-        <v>7032.0481000000009</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" ht="11.7" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="D52" s="10"/>
-      <c r="E52" s="9"/>
-    </row>
-    <row r="54" spans="1:6" ht="11.7" x14ac:dyDescent="0.4">
-      <c r="A54" s="62" t="s">
+      <c r="E55" s="71"/>
+      <c r="F55" s="46">
+        <f>SUM(F52+F53+F54)</f>
+        <v>7453.4911000000011</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" ht="11.7" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="D56" s="10"/>
+      <c r="E56" s="9"/>
+    </row>
+    <row r="58" spans="1:6" ht="11.7" x14ac:dyDescent="0.4">
+      <c r="A58" s="77" t="s">
         <v>15</v>
       </c>
-      <c r="B54" s="62"/>
-      <c r="C54" s="62"/>
-      <c r="E54" s="11"/>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A56" s="2" t="s">
+      <c r="B58" s="77"/>
+      <c r="C58" s="77"/>
+      <c r="E58" s="11"/>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A60" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D56" s="2" t="s">
+      <c r="D60" s="2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A59" s="4"/>
-      <c r="D59" s="17"/>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A61" s="4"/>
-      <c r="B61" s="4"/>
-      <c r="D61" s="4"/>
-      <c r="E61" s="4"/>
-      <c r="F61" s="4"/>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A62" s="39"/>
-      <c r="B62" s="4"/>
-      <c r="C62" s="4"/>
-      <c r="D62" s="4"/>
-    </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A63" s="40"/>
-      <c r="B63" s="40"/>
-      <c r="D63" s="40"/>
-      <c r="E63" s="40"/>
+      <c r="A63" s="4"/>
+      <c r="D63" s="17"/>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A65" s="4"/>
+      <c r="B65" s="4"/>
+      <c r="D65" s="4"/>
+      <c r="E65" s="4"/>
+      <c r="F65" s="4"/>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A66" s="39"/>
+      <c r="B66" s="4"/>
+      <c r="C66" s="4"/>
+      <c r="D66" s="4"/>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A67" s="40"/>
+      <c r="B67" s="40"/>
+      <c r="D67" s="40"/>
+      <c r="E67" s="40"/>
     </row>
   </sheetData>
-  <mergeCells count="40">
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="A40:B40"/>
-    <mergeCell ref="A41:B41"/>
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="A38:B38"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="A27:C27"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="D51:E51"/>
+  <mergeCells count="44">
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="A58:C58"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A48:B48"/>
+    <mergeCell ref="A49:B49"/>
+    <mergeCell ref="D52:E52"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="D54:E54"/>
+    <mergeCell ref="D55:E55"/>
     <mergeCell ref="A13:B13"/>
     <mergeCell ref="A14:B14"/>
     <mergeCell ref="A22:B22"/>
@@ -1806,26 +1931,23 @@
     <mergeCell ref="A36:B36"/>
     <mergeCell ref="A15:B15"/>
     <mergeCell ref="A16:B16"/>
-    <mergeCell ref="D49:E49"/>
-    <mergeCell ref="A54:C54"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="D53:E53"/>
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="A38:B38"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="A43:B43"/>
     <mergeCell ref="A44:B44"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="D48:E48"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="D50:E50"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="A41:B41"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="A27:C27"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A39:B39"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.15748031496062992" top="1.75" bottom="0.74803149606299213" header="0.15748031496062992" footer="0.18"/>
-  <pageSetup paperSize="9" scale="69" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="62" orientation="portrait" r:id="rId1"/>
   <headerFooter scaleWithDoc="0">
     <oddHeader>&amp;L&amp;G&amp;C&amp;"Arial,Vet"&amp;16&amp;K04+000HASHPEE NV&amp;9
 Lindelaan 34, 9000 Gent 

</xml_diff>